<commit_message>
Documentation: stellar map plans
</commit_message>
<xml_diff>
--- a/Unstable/StarFighter/Documentation/Factions.xlsx
+++ b/Unstable/StarFighter/Documentation/Factions.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="189">
   <si>
     <t>Faction</t>
   </si>
@@ -108,9 +108,6 @@
     <t>Swarm</t>
   </si>
   <si>
-    <t>Time keepers</t>
-  </si>
-  <si>
     <t>continuous oscillator shots (DNA patterns), time shifting</t>
   </si>
   <si>
@@ -133,13 +130,470 @@
   </si>
   <si>
     <t>Cavalry</t>
+  </si>
+  <si>
+    <t>HUB</t>
+  </si>
+  <si>
+    <t>Vanguard_V7</t>
+  </si>
+  <si>
+    <t>Vanguard_V6</t>
+  </si>
+  <si>
+    <t>Vanguard_V5</t>
+  </si>
+  <si>
+    <t>Vanguard_V4</t>
+  </si>
+  <si>
+    <t>Vanrguard_V3</t>
+  </si>
+  <si>
+    <t>Vanguard_HUB1</t>
+  </si>
+  <si>
+    <t>Vanguard_V2</t>
+  </si>
+  <si>
+    <t>Vanguard_V1</t>
+  </si>
+  <si>
+    <t>Vanguard_HUB0</t>
+  </si>
+  <si>
+    <t>Vanguard_HUB2</t>
+  </si>
+  <si>
+    <t>Vanguard_HUB3</t>
+  </si>
+  <si>
+    <t>Vanguard_HUB6</t>
+  </si>
+  <si>
+    <t>Vanguard_HUB5</t>
+  </si>
+  <si>
+    <t>Vanguard_HUB4</t>
+  </si>
+  <si>
+    <t>Vanguard_V8</t>
+  </si>
+  <si>
+    <t>Vanguard_V9</t>
+  </si>
+  <si>
+    <t>Vanguard_V10</t>
+  </si>
+  <si>
+    <t>Vanguard_V11</t>
+  </si>
+  <si>
+    <t>Vanguard_V12</t>
+  </si>
+  <si>
+    <t>Vanguard_H4</t>
+  </si>
+  <si>
+    <t>Vanguard_H3</t>
+  </si>
+  <si>
+    <t>Vanguard_H1</t>
+  </si>
+  <si>
+    <t>Vanguard_H2</t>
+  </si>
+  <si>
+    <t>Swarm_H1</t>
+  </si>
+  <si>
+    <t>Swarm_H2</t>
+  </si>
+  <si>
+    <t>Swarm_HUB1</t>
+  </si>
+  <si>
+    <t>Swarm_V1</t>
+  </si>
+  <si>
+    <t>Swarm_V2</t>
+  </si>
+  <si>
+    <t>Swarm_HUB2</t>
+  </si>
+  <si>
+    <t>Swarm_V3</t>
+  </si>
+  <si>
+    <t>Swarm_V4</t>
+  </si>
+  <si>
+    <t>Swarm_V5</t>
+  </si>
+  <si>
+    <t>Swarm_HUB3</t>
+  </si>
+  <si>
+    <t>Swarm_V6</t>
+  </si>
+  <si>
+    <t>Swarm_V7</t>
+  </si>
+  <si>
+    <t>Swarm_V8</t>
+  </si>
+  <si>
+    <t>Swarm_HUB4</t>
+  </si>
+  <si>
+    <t>Swarm_H3</t>
+  </si>
+  <si>
+    <t>Swarm_H4</t>
+  </si>
+  <si>
+    <t>Vanguard_H5</t>
+  </si>
+  <si>
+    <t>Vanguard_H6</t>
+  </si>
+  <si>
+    <t>Swarm_H5</t>
+  </si>
+  <si>
+    <t>Swarm_HUB5</t>
+  </si>
+  <si>
+    <t>Swarm_V9</t>
+  </si>
+  <si>
+    <t>Swarm_V10</t>
+  </si>
+  <si>
+    <t>Swarm_HUB6</t>
+  </si>
+  <si>
+    <t>Swarm_H6</t>
+  </si>
+  <si>
+    <t>Swarm_H7</t>
+  </si>
+  <si>
+    <t>Swarm_H8</t>
+  </si>
+  <si>
+    <t>Swarm_H9</t>
+  </si>
+  <si>
+    <t>Swarm_H10</t>
+  </si>
+  <si>
+    <t>Corsair_HUB0</t>
+  </si>
+  <si>
+    <t>Corsair_H1</t>
+  </si>
+  <si>
+    <t>Corsair_V1</t>
+  </si>
+  <si>
+    <t>Corsair_V2</t>
+  </si>
+  <si>
+    <t>Corsair_V3</t>
+  </si>
+  <si>
+    <t>Corsair_HUB1</t>
+  </si>
+  <si>
+    <t>Corsair_H2</t>
+  </si>
+  <si>
+    <t>Corsair_H3</t>
+  </si>
+  <si>
+    <t>Corsair_H4</t>
+  </si>
+  <si>
+    <t>Corsair_V4</t>
+  </si>
+  <si>
+    <t>Corsair_V5</t>
+  </si>
+  <si>
+    <t>Corsair_V6</t>
+  </si>
+  <si>
+    <t>Corsair_HUB2</t>
+  </si>
+  <si>
+    <t>Corsair_H7</t>
+  </si>
+  <si>
+    <t>Corsair_HUB3</t>
+  </si>
+  <si>
+    <t>Corsair_HUB4</t>
+  </si>
+  <si>
+    <t>Corsair_V7</t>
+  </si>
+  <si>
+    <t>Corsair_V8</t>
+  </si>
+  <si>
+    <t>Corsair_V9</t>
+  </si>
+  <si>
+    <t>Corsair_HUB5</t>
+  </si>
+  <si>
+    <t>Corsair_HUB6</t>
+  </si>
+  <si>
+    <t>Corsair_HUB7</t>
+  </si>
+  <si>
+    <t>Corsair_H_Highway</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Corsair_V_Highway</t>
+  </si>
+  <si>
+    <t>Corsair_H8</t>
+  </si>
+  <si>
+    <t>Corsair_H9</t>
+  </si>
+  <si>
+    <t>Corsair_H10</t>
+  </si>
+  <si>
+    <t>Corsair_HUB8</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>Corsair</t>
+  </si>
+  <si>
+    <t>Corsair_H11</t>
+  </si>
+  <si>
+    <t>Vanguard_V13</t>
+  </si>
+  <si>
+    <t>Vanguard_V14</t>
+  </si>
+  <si>
+    <t>Vanguard_V15</t>
+  </si>
+  <si>
+    <t>^^^[locked]&lt;&lt;&lt;</t>
+  </si>
+  <si>
+    <t>^^^[locked]</t>
+  </si>
+  <si>
+    <t>Royal_V1</t>
+  </si>
+  <si>
+    <t>Royal_V2</t>
+  </si>
+  <si>
+    <t>Royal_V3</t>
+  </si>
+  <si>
+    <t>Royal_HUB1</t>
+  </si>
+  <si>
+    <t>Royal_V4</t>
+  </si>
+  <si>
+    <t>Royal_V5</t>
+  </si>
+  <si>
+    <t>Royal_HUB2</t>
+  </si>
+  <si>
+    <t>Royal_H1</t>
+  </si>
+  <si>
+    <t>Royal_H2</t>
+  </si>
+  <si>
+    <t>Royal_HUB4</t>
+  </si>
+  <si>
+    <t>Royal_V6</t>
+  </si>
+  <si>
+    <t>Royal_V7</t>
+  </si>
+  <si>
+    <t>Royal_V8</t>
+  </si>
+  <si>
+    <t>Royal_HUB3</t>
+  </si>
+  <si>
+    <t>Royal_HUB5</t>
+  </si>
+  <si>
+    <t>Royal_HUB6</t>
+  </si>
+  <si>
+    <t>Royal_H3</t>
+  </si>
+  <si>
+    <t>Royal_H4</t>
+  </si>
+  <si>
+    <t>Royal_H5</t>
+  </si>
+  <si>
+    <t>Royal_H6</t>
+  </si>
+  <si>
+    <t>Royal_H_Highway</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Swarm_V_Highway</t>
+  </si>
+  <si>
+    <t>Royal_V9</t>
+  </si>
+  <si>
+    <t>Royal_V10</t>
+  </si>
+  <si>
+    <t>Royal_V11</t>
+  </si>
+  <si>
+    <t>Royal_V12</t>
+  </si>
+  <si>
+    <t>Royal_V13</t>
+  </si>
+  <si>
+    <t>Royal_HUB7</t>
+  </si>
+  <si>
+    <t>Royal</t>
+  </si>
+  <si>
+    <t>Anciants</t>
+  </si>
+  <si>
+    <t>Anciant_H1</t>
+  </si>
+  <si>
+    <t>Anciant_H2</t>
+  </si>
+  <si>
+    <t>Anciant_HUB1</t>
+  </si>
+  <si>
+    <t>Anciant_V1</t>
+  </si>
+  <si>
+    <t>Anciant_V2</t>
+  </si>
+  <si>
+    <t>Anciant_HUB2</t>
+  </si>
+  <si>
+    <t>Anciant_V3</t>
+  </si>
+  <si>
+    <t>Anciant_V4</t>
+  </si>
+  <si>
+    <t>Anciant_HUB3</t>
+  </si>
+  <si>
+    <t>Anciant_H4</t>
+  </si>
+  <si>
+    <t>Anciant_HUB4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Anciant_V_Highway</t>
+  </si>
+  <si>
+    <t>Anciant_V5</t>
+  </si>
+  <si>
+    <t>Anciant_V6</t>
+  </si>
+  <si>
+    <t>Anciant_V7</t>
+  </si>
+  <si>
+    <t>Anciant_HUB5</t>
+  </si>
+  <si>
+    <t>Anciant_HUB6</t>
+  </si>
+  <si>
+    <t>Anciant_HUB8</t>
+  </si>
+  <si>
+    <t>Anciant_H5</t>
+  </si>
+  <si>
+    <t>Anciant_H6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Royal_V_Highway</t>
+  </si>
+  <si>
+    <t>Anciant_V8</t>
+  </si>
+  <si>
+    <t>Anciant_H8</t>
+  </si>
+  <si>
+    <t>Anciant_V9</t>
+  </si>
+  <si>
+    <t>Anciant_V10</t>
+  </si>
+  <si>
+    <t>AnciantH3</t>
+  </si>
+  <si>
+    <t>Anciant_H7</t>
+  </si>
+  <si>
+    <t>Neutral_HUB</t>
+  </si>
+  <si>
+    <t>Anciant_V11</t>
+  </si>
+  <si>
+    <t>Neutral</t>
+  </si>
+  <si>
+    <t>Zones combat</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,8 +617,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -201,8 +662,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -366,11 +839,100 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -414,15 +976,156 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -432,35 +1135,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -470,8 +1149,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFFF66"/>
       <color rgb="FFFFC91D"/>
-      <color rgb="FFFFFF66"/>
     </mruColors>
   </colors>
   <extLst>
@@ -769,10 +1448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:T57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="C10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N51" sqref="N51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -780,129 +1459,128 @@
     <col min="1" max="1" width="13.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="52" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="63" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="14.5703125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="16.5703125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="15.28515625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="15.7109375" style="1" customWidth="1"/>
-    <col min="16" max="16" width="15.42578125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="15.140625" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="28"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
+      <c r="P1" s="60"/>
+      <c r="Q1" s="61"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="26" t="s">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="H2" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="25" t="s">
+      <c r="I2" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="24" t="s">
+      <c r="J2" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="25" t="s">
+      <c r="K2" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="24" t="s">
+      <c r="L2" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="26" t="s">
+      <c r="M2" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="24" t="s">
+      <c r="N2" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="O2" s="25" t="s">
+      <c r="O2" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="P2" s="24" t="s">
+      <c r="P2" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="25" t="s">
+      <c r="Q2" s="19" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="30" t="s">
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="17"/>
-      <c r="F3" s="16" t="s">
+      <c r="E3" s="63"/>
+      <c r="F3" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="17"/>
-      <c r="H3" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="I3" s="17"/>
-      <c r="J3" s="18" t="s">
+      <c r="G3" s="63"/>
+      <c r="H3" s="64" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" s="63"/>
+      <c r="J3" s="65" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="19"/>
-      <c r="L3" s="18" t="s">
+      <c r="K3" s="66"/>
+      <c r="L3" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="20"/>
-      <c r="N3" s="18" t="s">
+      <c r="M3" s="67"/>
+      <c r="N3" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="19"/>
-      <c r="P3" s="16" t="s">
+      <c r="O3" s="66"/>
+      <c r="P3" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="Q3" s="17"/>
+      <c r="Q3" s="63"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
@@ -919,14 +1597,14 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="21"/>
+      <c r="I4" s="15"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="3"/>
       <c r="M4" s="2"/>
-      <c r="N4" s="21"/>
+      <c r="N4" s="15"/>
       <c r="O4" s="4"/>
-      <c r="P4" s="21"/>
+      <c r="P4" s="15"/>
       <c r="Q4" s="4"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -934,24 +1612,24 @@
         <v>29</v>
       </c>
       <c r="B5" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>33</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>34</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
-      <c r="I5" s="22"/>
+      <c r="I5" s="16"/>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
       <c r="L5" s="6"/>
       <c r="M5" s="5"/>
-      <c r="N5" s="22"/>
+      <c r="N5" s="16"/>
       <c r="O5" s="7"/>
-      <c r="P5" s="22"/>
+      <c r="P5" s="16"/>
       <c r="Q5" s="7"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -969,64 +1647,64 @@
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
-      <c r="I6" s="22"/>
+      <c r="I6" s="16"/>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
       <c r="L6" s="6"/>
       <c r="M6" s="5"/>
-      <c r="N6" s="22"/>
+      <c r="N6" s="16"/>
       <c r="O6" s="7"/>
-      <c r="P6" s="22"/>
+      <c r="P6" s="16"/>
       <c r="Q6" s="7"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="39" t="s">
+        <v>156</v>
+      </c>
+      <c r="B7" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="C7" s="39" t="s">
         <v>31</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>32</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
-      <c r="I7" s="22"/>
+      <c r="I7" s="16"/>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
       <c r="L7" s="6"/>
       <c r="M7" s="5"/>
-      <c r="N7" s="22"/>
+      <c r="N7" s="16"/>
       <c r="O7" s="7"/>
-      <c r="P7" s="22"/>
+      <c r="P7" s="16"/>
       <c r="Q7" s="7"/>
     </row>
     <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="14" t="s">
         <v>35</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>36</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
-      <c r="I8" s="23"/>
+      <c r="I8" s="17"/>
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
       <c r="L8" s="9"/>
       <c r="M8" s="8"/>
-      <c r="N8" s="23"/>
+      <c r="N8" s="17"/>
       <c r="O8" s="10"/>
-      <c r="P8" s="23"/>
+      <c r="P8" s="17"/>
       <c r="Q8" s="10"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -1073,8 +1751,689 @@
         <v>14</v>
       </c>
     </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M13" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="P13" s="22" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M14" s="40" t="s">
+        <v>139</v>
+      </c>
+      <c r="P14" s="40" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M15" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="P15" s="30" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M16" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="P16" s="30" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="17" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="D17" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="E17" s="52" t="s">
+        <v>147</v>
+      </c>
+      <c r="F17" s="53"/>
+      <c r="G17" s="53"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="53"/>
+      <c r="J17" s="27" t="s">
+        <v>154</v>
+      </c>
+      <c r="K17" s="43" t="s">
+        <v>146</v>
+      </c>
+      <c r="L17" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="N17" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="O17" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="P17" s="22" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="4:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="45" t="s">
+        <v>177</v>
+      </c>
+      <c r="J18" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="M18" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="P18" s="30" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="19" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="D19" s="46"/>
+      <c r="G19" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="J19" s="44" t="s">
+        <v>180</v>
+      </c>
+      <c r="M19" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="P19" s="30" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="20" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="D20" s="46"/>
+      <c r="G20" s="41" t="s">
+        <v>170</v>
+      </c>
+      <c r="J20" s="29" t="s">
+        <v>178</v>
+      </c>
+      <c r="M20" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="N20" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="O20" s="40" t="s">
+        <v>135</v>
+      </c>
+      <c r="P20" s="22" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="21" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="D21" s="47"/>
+      <c r="G21" s="29" t="s">
+        <v>169</v>
+      </c>
+      <c r="J21" s="29" t="s">
+        <v>171</v>
+      </c>
+      <c r="M21" s="30" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="D22" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="E22" s="29" t="s">
+        <v>176</v>
+      </c>
+      <c r="F22" s="29" t="s">
+        <v>175</v>
+      </c>
+      <c r="G22" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="H22" s="29" t="s">
+        <v>182</v>
+      </c>
+      <c r="I22" s="29" t="s">
+        <v>166</v>
+      </c>
+      <c r="J22" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="M22" s="30" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="G23" s="41" t="s">
+        <v>164</v>
+      </c>
+      <c r="J23" s="42" t="s">
+        <v>184</v>
+      </c>
+      <c r="M23" s="30" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="G24" s="29" t="s">
+        <v>163</v>
+      </c>
+      <c r="J24" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="K24" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="L24" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="M24" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="N24" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="O24" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="P24" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="T24" s="22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="G25" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="J25" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="M25" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="P25" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="T25" s="28" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="G26" s="29" t="s">
+        <v>161</v>
+      </c>
+      <c r="J26" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="M26" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="P26" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="T26" s="38" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="G27" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="J27" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="M27" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="P27" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q27" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="R27" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="S27" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="T27" s="27" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="G28" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="H28" s="29" t="s">
+        <v>158</v>
+      </c>
+      <c r="I28" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="J28" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="K28" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="L28" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="M28" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="P28" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="T28" s="33" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="29" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="G29" s="29" t="s">
+        <v>181</v>
+      </c>
+      <c r="J29" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="M29" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="P29" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="T29" s="51" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="30" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="G30" s="41" t="s">
+        <v>185</v>
+      </c>
+      <c r="J30" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="M30" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="P30" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="T30" s="49"/>
+    </row>
+    <row r="31" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="G31" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="J31" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="K31" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="L31" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="M31" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="N31" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="O31" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="P31" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="T31" s="49"/>
+    </row>
+    <row r="32" spans="4:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G32" s="48" t="s">
+        <v>168</v>
+      </c>
+      <c r="J32" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="P32" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="T32" s="49"/>
+    </row>
+    <row r="33" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G33" s="49"/>
+      <c r="J33" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="P33" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="T33" s="49"/>
+    </row>
+    <row r="34" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G34" s="49"/>
+      <c r="J34" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="P34" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="T34" s="49"/>
+    </row>
+    <row r="35" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G35" s="49"/>
+      <c r="J35" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="K35" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="L35" s="22" t="s">
+        <v>90</v>
+      </c>
+      <c r="M35" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="N35" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="O35" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="P35" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="T35" s="49"/>
+    </row>
+    <row r="36" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G36" s="49"/>
+      <c r="J36" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="L36" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="T36" s="49"/>
+    </row>
+    <row r="37" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G37" s="49"/>
+      <c r="J37" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="L37" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="T37" s="49"/>
+    </row>
+    <row r="38" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G38" s="50"/>
+      <c r="J38" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="L38" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="T38" s="49"/>
+    </row>
+    <row r="39" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G39" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="H39" s="29" t="s">
+        <v>183</v>
+      </c>
+      <c r="I39" s="41" t="s">
+        <v>179</v>
+      </c>
+      <c r="J39" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="L39" s="22" t="s">
+        <v>95</v>
+      </c>
+      <c r="M39" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="N39" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="O39" s="36" t="s">
+        <v>98</v>
+      </c>
+      <c r="P39" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="T39" s="49"/>
+    </row>
+    <row r="40" spans="7:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J40" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="L40" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="T40" s="49"/>
+    </row>
+    <row r="41" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="J41" s="55"/>
+      <c r="L41" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="T41" s="49"/>
+    </row>
+    <row r="42" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="J42" s="55"/>
+      <c r="L42" s="36" t="s">
+        <v>101</v>
+      </c>
+      <c r="T42" s="50"/>
+    </row>
+    <row r="43" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="J43" s="55"/>
+      <c r="L43" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="M43" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="N43" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="O43" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="P43" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q43" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="R43" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="S43" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="T43" s="42" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="44" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="J44" s="55"/>
+      <c r="O44" s="31" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="45" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="J45" s="55"/>
+      <c r="O45" s="31" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="46" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="J46" s="56"/>
+      <c r="O46" s="36" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="47" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="J47" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="K47" s="57" t="s">
+        <v>112</v>
+      </c>
+      <c r="L47" s="58"/>
+      <c r="M47" s="58"/>
+      <c r="N47" s="59"/>
+      <c r="O47" s="22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="50" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="J50" s="26" t="s">
+        <v>187</v>
+      </c>
+      <c r="K50" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="L50" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="M50" s="34" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="51" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I51" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="J51" s="24">
+        <v>21</v>
+      </c>
+      <c r="K51" s="24">
+        <v>15</v>
+      </c>
+      <c r="L51" s="24">
+        <v>6</v>
+      </c>
+      <c r="M51" s="24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I52" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="J52" s="25">
+        <v>21</v>
+      </c>
+      <c r="K52" s="25">
+        <v>11</v>
+      </c>
+      <c r="L52" s="25">
+        <v>10</v>
+      </c>
+      <c r="M52" s="25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I53" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="J53" s="31">
+        <v>22</v>
+      </c>
+      <c r="K53" s="31">
+        <v>10</v>
+      </c>
+      <c r="L53" s="31">
+        <v>12</v>
+      </c>
+      <c r="M53" s="31">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I54" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="J54" s="30">
+        <v>20</v>
+      </c>
+      <c r="K54" s="30">
+        <v>13</v>
+      </c>
+      <c r="L54" s="30">
+        <v>7</v>
+      </c>
+      <c r="M54" s="30">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I55" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="J55" s="29">
+        <v>20</v>
+      </c>
+      <c r="K55" s="29">
+        <v>12</v>
+      </c>
+      <c r="L55" s="29">
+        <v>8</v>
+      </c>
+      <c r="M55" s="29">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I56" s="42" t="s">
+        <v>186</v>
+      </c>
+      <c r="J56" s="42">
+        <v>0</v>
+      </c>
+      <c r="K56" s="42">
+        <v>0</v>
+      </c>
+      <c r="L56" s="42">
+        <v>0</v>
+      </c>
+      <c r="M56" s="42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="9:13" x14ac:dyDescent="0.25">
+      <c r="I57" s="68" t="s">
+        <v>188</v>
+      </c>
+      <c r="J57" s="69">
+        <f>SUM(J51:J56)</f>
+        <v>104</v>
+      </c>
+      <c r="K57" s="69">
+        <f>SUM(K51:K56)</f>
+        <v>61</v>
+      </c>
+      <c r="L57" s="69">
+        <f>SUM(L51:L56)</f>
+        <v>43</v>
+      </c>
+      <c r="M57" s="69">
+        <f>SUM(M51:M56)</f>
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="14">
+    <mergeCell ref="K47:N47"/>
     <mergeCell ref="D1:Q1"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="F3:G3"/>
@@ -1083,6 +2442,11 @@
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="G32:G38"/>
+    <mergeCell ref="T29:T42"/>
+    <mergeCell ref="E17:I17"/>
+    <mergeCell ref="J40:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Placeholder assets for Vanguard enemies + doc
</commit_message>
<xml_diff>
--- a/Unstable/StarFighter/Documentation/Factions.xlsx
+++ b/Unstable/StarFighter/Documentation/Factions.xlsx
@@ -78,9 +78,6 @@
     <t>Big combat</t>
   </si>
   <si>
-    <t>Glass canon</t>
-  </si>
-  <si>
     <t>Omega</t>
   </si>
   <si>
@@ -587,6 +584,9 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Glass cannon</t>
   </si>
 </sst>
 </file>
@@ -1066,6 +1066,45 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1101,45 +1140,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1450,8 +1450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N51" sqref="N51"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1485,22 +1485,22 @@
       <c r="C1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="60" t="s">
+      <c r="D1" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
-      <c r="O1" s="60"/>
-      <c r="P1" s="60"/>
-      <c r="Q1" s="61"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
+      <c r="P1" s="50"/>
+      <c r="Q1" s="51"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
@@ -1537,10 +1537,10 @@
         <v>17</v>
       </c>
       <c r="N2" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="19" t="s">
         <v>21</v>
-      </c>
-      <c r="O2" s="19" t="s">
-        <v>22</v>
       </c>
       <c r="P2" s="18" t="s">
         <v>15</v>
@@ -1553,34 +1553,34 @@
       <c r="A3" s="16"/>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
-      <c r="D3" s="62" t="s">
+      <c r="D3" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="63"/>
-      <c r="F3" s="64" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="63"/>
-      <c r="H3" s="64" t="s">
-        <v>37</v>
-      </c>
-      <c r="I3" s="63"/>
-      <c r="J3" s="65" t="s">
+      <c r="E3" s="53"/>
+      <c r="F3" s="54" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="53"/>
+      <c r="H3" s="54" t="s">
+        <v>188</v>
+      </c>
+      <c r="I3" s="53"/>
+      <c r="J3" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="66"/>
-      <c r="L3" s="65" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" s="67"/>
-      <c r="N3" s="65" t="s">
+      <c r="K3" s="56"/>
+      <c r="L3" s="55" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="57"/>
+      <c r="N3" s="55" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" s="56"/>
+      <c r="P3" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="66"/>
-      <c r="P3" s="64" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q3" s="63"/>
+      <c r="Q3" s="53"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
@@ -1609,13 +1609,13 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>32</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>33</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
@@ -1634,13 +1634,13 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="C6" s="13" t="s">
         <v>27</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>28</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
@@ -1659,13 +1659,13 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="39" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B7" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="39" t="s">
         <v>30</v>
-      </c>
-      <c r="C7" s="39" t="s">
-        <v>31</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
@@ -1684,13 +1684,13 @@
     </row>
     <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="14" t="s">
         <v>34</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>35</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
@@ -1753,559 +1753,559 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="M13" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="P13" s="22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="M14" s="40" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="P14" s="40" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="M15" s="30" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="P15" s="30" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="M16" s="30" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="P16" s="30" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D17" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="E17" s="52" t="s">
-        <v>147</v>
-      </c>
-      <c r="F17" s="53"/>
-      <c r="G17" s="53"/>
-      <c r="H17" s="53"/>
-      <c r="I17" s="53"/>
+        <v>153</v>
+      </c>
+      <c r="E17" s="65" t="s">
+        <v>146</v>
+      </c>
+      <c r="F17" s="66"/>
+      <c r="G17" s="66"/>
+      <c r="H17" s="66"/>
+      <c r="I17" s="66"/>
       <c r="J17" s="27" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K17" s="43" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L17" s="30" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="M17" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="N17" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="O17" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="P17" s="22" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="18" spans="4:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="58" t="s">
+        <v>176</v>
+      </c>
+      <c r="J18" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="M18" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="P18" s="30" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="19" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="D19" s="59"/>
+      <c r="G19" s="22" t="s">
+        <v>166</v>
+      </c>
+      <c r="J19" s="44" t="s">
+        <v>179</v>
+      </c>
+      <c r="M19" s="30" t="s">
+        <v>130</v>
+      </c>
+      <c r="P19" s="30" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="20" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="D20" s="59"/>
+      <c r="G20" s="41" t="s">
+        <v>169</v>
+      </c>
+      <c r="J20" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="M20" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="N20" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="N17" s="30" t="s">
-        <v>143</v>
-      </c>
-      <c r="O17" s="30" t="s">
-        <v>144</v>
-      </c>
-      <c r="P17" s="22" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="18" spans="4:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D18" s="45" t="s">
-        <v>177</v>
-      </c>
-      <c r="J18" s="33" t="s">
-        <v>126</v>
-      </c>
-      <c r="M18" s="30" t="s">
-        <v>132</v>
-      </c>
-      <c r="P18" s="30" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="19" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="D19" s="46"/>
-      <c r="G19" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="J19" s="44" t="s">
-        <v>180</v>
-      </c>
-      <c r="M19" s="30" t="s">
-        <v>131</v>
-      </c>
-      <c r="P19" s="30" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="20" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="D20" s="46"/>
-      <c r="G20" s="41" t="s">
+      <c r="O20" s="40" t="s">
+        <v>134</v>
+      </c>
+      <c r="P20" s="22" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="21" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="D21" s="60"/>
+      <c r="G21" s="29" t="s">
+        <v>168</v>
+      </c>
+      <c r="J21" s="29" t="s">
         <v>170</v>
       </c>
-      <c r="J20" s="29" t="s">
-        <v>178</v>
-      </c>
-      <c r="M20" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="N20" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="O20" s="40" t="s">
-        <v>135</v>
-      </c>
-      <c r="P20" s="22" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="21" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="D21" s="47"/>
-      <c r="G21" s="29" t="s">
-        <v>169</v>
-      </c>
-      <c r="J21" s="29" t="s">
-        <v>171</v>
-      </c>
       <c r="M21" s="30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" spans="4:20" x14ac:dyDescent="0.25">
       <c r="D22" s="22" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E22" s="29" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F22" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G22" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="H22" s="29" t="s">
+        <v>181</v>
+      </c>
+      <c r="I22" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="H22" s="29" t="s">
-        <v>182</v>
-      </c>
-      <c r="I22" s="29" t="s">
-        <v>166</v>
-      </c>
       <c r="J22" s="22" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M22" s="30" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="4:20" x14ac:dyDescent="0.25">
       <c r="G23" s="41" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="J23" s="42" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="M23" s="30" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="4:20" x14ac:dyDescent="0.25">
       <c r="G24" s="29" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J24" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="K24" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="L24" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="M24" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="K24" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="L24" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="M24" s="22" t="s">
-        <v>50</v>
-      </c>
       <c r="N24" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="O24" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="O24" s="25" t="s">
+      <c r="P24" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="P24" s="22" t="s">
-        <v>64</v>
-      </c>
       <c r="T24" s="22" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="4:20" x14ac:dyDescent="0.25">
       <c r="G25" s="22" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="J25" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M25" s="23" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P25" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="T25" s="28" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" spans="4:20" x14ac:dyDescent="0.25">
       <c r="G26" s="29" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J26" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M26" s="24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P26" s="25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T26" s="38" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="4:20" x14ac:dyDescent="0.25">
       <c r="G27" s="29" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J27" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M27" s="24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="P27" s="22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q27" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="R27" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="R27" s="25" t="s">
-        <v>77</v>
-      </c>
       <c r="S27" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="T27" s="27" t="s">
         <v>80</v>
-      </c>
-      <c r="T27" s="27" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="28" spans="4:20" x14ac:dyDescent="0.25">
       <c r="G28" s="22" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H28" s="29" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I28" s="29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="J28" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K28" s="24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L28" s="24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M28" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P28" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="T28" s="33" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="29" spans="4:20" x14ac:dyDescent="0.25">
       <c r="G29" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J29" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M29" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P29" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="T29" s="51" t="s">
-        <v>148</v>
+        <v>68</v>
+      </c>
+      <c r="T29" s="64" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="30" spans="4:20" x14ac:dyDescent="0.25">
       <c r="G30" s="41" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J30" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M30" s="24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P30" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="T30" s="49"/>
+        <v>69</v>
+      </c>
+      <c r="T30" s="62"/>
     </row>
     <row r="31" spans="4:20" x14ac:dyDescent="0.25">
       <c r="G31" s="22" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="J31" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="K31" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="L31" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="M31" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="N31" s="25" t="s">
+        <v>84</v>
+      </c>
+      <c r="O31" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="P31" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="T31" s="62"/>
+    </row>
+    <row r="32" spans="4:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G32" s="61" t="s">
+        <v>167</v>
+      </c>
+      <c r="J32" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="K31" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="L31" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="M31" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="N31" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="O31" s="25" t="s">
+      <c r="P32" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="T32" s="62"/>
+    </row>
+    <row r="33" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G33" s="62"/>
+      <c r="J33" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="P33" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="T33" s="62"/>
+    </row>
+    <row r="34" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G34" s="62"/>
+      <c r="J34" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="P34" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="T34" s="62"/>
+    </row>
+    <row r="35" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G35" s="62"/>
+      <c r="J35" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="K35" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="L35" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="M35" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="N35" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="O35" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="P31" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="T31" s="49"/>
-    </row>
-    <row r="32" spans="4:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G32" s="48" t="s">
-        <v>168</v>
-      </c>
-      <c r="J32" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="P32" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="T32" s="49"/>
-    </row>
-    <row r="33" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="G33" s="49"/>
-      <c r="J33" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="P33" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="T33" s="49"/>
-    </row>
-    <row r="34" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="G34" s="49"/>
-      <c r="J34" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="P34" s="28" t="s">
+      <c r="P35" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="T34" s="49"/>
-    </row>
-    <row r="35" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="G35" s="49"/>
-      <c r="J35" s="33" t="s">
-        <v>125</v>
-      </c>
-      <c r="K35" s="31" t="s">
+      <c r="T35" s="62"/>
+    </row>
+    <row r="36" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G36" s="62"/>
+      <c r="J36" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="L36" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="L35" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="M35" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="N35" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="O35" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="P35" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="T35" s="49"/>
-    </row>
-    <row r="36" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="G36" s="49"/>
-      <c r="J36" s="24" t="s">
-        <v>124</v>
-      </c>
-      <c r="L36" s="31" t="s">
+      <c r="T36" s="62"/>
+    </row>
+    <row r="37" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G37" s="62"/>
+      <c r="J37" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="L37" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="T36" s="49"/>
-    </row>
-    <row r="37" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="G37" s="49"/>
-      <c r="J37" s="24" t="s">
-        <v>123</v>
-      </c>
-      <c r="L37" s="31" t="s">
+      <c r="T37" s="62"/>
+    </row>
+    <row r="38" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="G38" s="63"/>
+      <c r="J38" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="L38" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="T37" s="49"/>
-    </row>
-    <row r="38" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="G38" s="50"/>
-      <c r="J38" s="24" t="s">
-        <v>122</v>
-      </c>
-      <c r="L38" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="T38" s="49"/>
+      <c r="T38" s="62"/>
     </row>
     <row r="39" spans="7:20" x14ac:dyDescent="0.25">
       <c r="G39" s="22" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H39" s="29" t="s">
+        <v>182</v>
+      </c>
+      <c r="I39" s="41" t="s">
+        <v>178</v>
+      </c>
+      <c r="J39" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="L39" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="M39" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="N39" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="O39" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="P39" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="T39" s="62"/>
+    </row>
+    <row r="40" spans="7:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J40" s="67" t="s">
+        <v>112</v>
+      </c>
+      <c r="L40" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="T40" s="62"/>
+    </row>
+    <row r="41" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="J41" s="68"/>
+      <c r="L41" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="T41" s="62"/>
+    </row>
+    <row r="42" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="J42" s="68"/>
+      <c r="L42" s="36" t="s">
+        <v>100</v>
+      </c>
+      <c r="T42" s="63"/>
+    </row>
+    <row r="43" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="J43" s="68"/>
+      <c r="L43" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="M43" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="N43" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="O43" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="P43" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q43" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="R43" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="S43" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="T43" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="I39" s="41" t="s">
-        <v>179</v>
-      </c>
-      <c r="J39" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="L39" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="M39" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="N39" s="31" t="s">
-        <v>97</v>
-      </c>
-      <c r="O39" s="36" t="s">
-        <v>98</v>
-      </c>
-      <c r="P39" s="22" t="s">
-        <v>104</v>
-      </c>
-      <c r="T39" s="49"/>
-    </row>
-    <row r="40" spans="7:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J40" s="54" t="s">
-        <v>113</v>
-      </c>
-      <c r="L40" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="T40" s="49"/>
-    </row>
-    <row r="41" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="J41" s="55"/>
-      <c r="L41" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="T41" s="49"/>
-    </row>
-    <row r="42" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="J42" s="55"/>
-      <c r="L42" s="36" t="s">
-        <v>101</v>
-      </c>
-      <c r="T42" s="50"/>
-    </row>
-    <row r="43" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="J43" s="55"/>
-      <c r="L43" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="M43" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="N43" s="31" t="s">
-        <v>114</v>
-      </c>
-      <c r="O43" s="22" t="s">
+    </row>
+    <row r="44" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="J44" s="68"/>
+      <c r="O44" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="P43" s="31" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q43" s="31" t="s">
-        <v>116</v>
-      </c>
-      <c r="R43" s="36" t="s">
-        <v>121</v>
-      </c>
-      <c r="S43" s="35" t="s">
-        <v>110</v>
-      </c>
-      <c r="T43" s="42" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="44" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="J44" s="55"/>
-      <c r="O44" s="31" t="s">
+    </row>
+    <row r="45" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="J45" s="68"/>
+      <c r="O45" s="31" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="45" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="J45" s="55"/>
-      <c r="O45" s="31" t="s">
+    <row r="46" spans="7:20" x14ac:dyDescent="0.25">
+      <c r="J46" s="69"/>
+      <c r="O46" s="36" t="s">
         <v>107</v>
-      </c>
-    </row>
-    <row r="46" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="J46" s="56"/>
-      <c r="O46" s="36" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="47" spans="7:20" x14ac:dyDescent="0.25">
       <c r="J47" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="K47" s="47" t="s">
         <v>111</v>
       </c>
-      <c r="K47" s="57" t="s">
-        <v>112</v>
-      </c>
-      <c r="L47" s="58"/>
-      <c r="M47" s="58"/>
-      <c r="N47" s="59"/>
+      <c r="L47" s="48"/>
+      <c r="M47" s="48"/>
+      <c r="N47" s="49"/>
       <c r="O47" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="50" spans="9:13" x14ac:dyDescent="0.25">
       <c r="J50" s="26" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="K50" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="L50" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="L50" s="22" t="s">
-        <v>119</v>
-      </c>
       <c r="M50" s="34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="51" spans="9:13" x14ac:dyDescent="0.25">
@@ -2327,7 +2327,7 @@
     </row>
     <row r="52" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I52" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J52" s="25">
         <v>21</v>
@@ -2344,7 +2344,7 @@
     </row>
     <row r="53" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I53" s="31" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J53" s="31">
         <v>22</v>
@@ -2361,7 +2361,7 @@
     </row>
     <row r="54" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I54" s="30" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J54" s="30">
         <v>20</v>
@@ -2378,7 +2378,7 @@
     </row>
     <row r="55" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I55" s="29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J55" s="29">
         <v>20</v>
@@ -2395,7 +2395,7 @@
     </row>
     <row r="56" spans="9:13" x14ac:dyDescent="0.25">
       <c r="I56" s="42" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J56" s="42">
         <v>0</v>
@@ -2411,28 +2411,31 @@
       </c>
     </row>
     <row r="57" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I57" s="68" t="s">
-        <v>188</v>
-      </c>
-      <c r="J57" s="69">
+      <c r="I57" s="45" t="s">
+        <v>187</v>
+      </c>
+      <c r="J57" s="46">
         <f>SUM(J51:J56)</f>
         <v>104</v>
       </c>
-      <c r="K57" s="69">
+      <c r="K57" s="46">
         <f>SUM(K51:K56)</f>
         <v>61</v>
       </c>
-      <c r="L57" s="69">
+      <c r="L57" s="46">
         <f>SUM(L51:L56)</f>
         <v>43</v>
       </c>
-      <c r="M57" s="69">
+      <c r="M57" s="46">
         <f>SUM(M51:M56)</f>
         <v>40</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="T29:T42"/>
+    <mergeCell ref="E17:I17"/>
+    <mergeCell ref="J40:J46"/>
     <mergeCell ref="K47:N47"/>
     <mergeCell ref="D1:Q1"/>
     <mergeCell ref="D3:E3"/>
@@ -2444,9 +2447,6 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="D18:D21"/>
     <mergeCell ref="G32:G38"/>
-    <mergeCell ref="T29:T42"/>
-    <mergeCell ref="E17:I17"/>
-    <mergeCell ref="J40:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixing dipersion on alternate shots for enemies + Vanguard Beta1 integration
</commit_message>
<xml_diff>
--- a/Unstable/StarFighter/Documentation/Factions.xlsx
+++ b/Unstable/StarFighter/Documentation/Factions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="195">
   <si>
     <t>Faction</t>
   </si>
@@ -587,6 +587,24 @@
   </si>
   <si>
     <t>Glass cannon</t>
+  </si>
+  <si>
+    <t>Sigma</t>
+  </si>
+  <si>
+    <t>Sigma'</t>
+  </si>
+  <si>
+    <t>Station Prométhée (Canon intergalactique)</t>
+  </si>
+  <si>
+    <t>Amiral Brethus (Battlecruiser)</t>
+  </si>
+  <si>
+    <t>Capitaine Elias (Flotte d'interception)</t>
+  </si>
+  <si>
+    <t>Commandante Astride (Chef de l'Avant-Garde)</t>
   </si>
 </sst>
 </file>
@@ -932,7 +950,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1072,6 +1090,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1117,29 +1159,17 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1448,34 +1478,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T57"/>
+  <dimension ref="A1:V57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="52" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="63" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="5" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -1485,24 +1517,26 @@
       <c r="C1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
-      <c r="O1" s="50"/>
-      <c r="P1" s="50"/>
-      <c r="Q1" s="51"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="59"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -1512,77 +1546,85 @@
       <c r="E2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="H2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="I2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="J2" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="K2" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="L2" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="19" t="s">
+      <c r="M2" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="18" t="s">
+      <c r="N2" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="20" t="s">
+      <c r="O2" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="18" t="s">
+      <c r="P2" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="19" t="s">
+      <c r="Q2" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="P2" s="18" t="s">
+      <c r="R2" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="19" t="s">
+      <c r="S2" s="19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
-      <c r="D3" s="52" t="s">
+      <c r="D3" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="53"/>
-      <c r="F3" s="54" t="s">
+      <c r="E3" s="61"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="53"/>
-      <c r="H3" s="54" t="s">
+      <c r="I3" s="61"/>
+      <c r="J3" s="62" t="s">
         <v>188</v>
       </c>
-      <c r="I3" s="53"/>
-      <c r="J3" s="55" t="s">
+      <c r="K3" s="61"/>
+      <c r="L3" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="56"/>
-      <c r="L3" s="55" t="s">
+      <c r="M3" s="64"/>
+      <c r="N3" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="M3" s="57"/>
-      <c r="N3" s="55" t="s">
+      <c r="O3" s="65"/>
+      <c r="P3" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="O3" s="56"/>
-      <c r="P3" s="54" t="s">
+      <c r="Q3" s="64"/>
+      <c r="R3" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="Q3" s="53"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="S3" s="61"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>1</v>
       </c>
@@ -1594,20 +1636,22 @@
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="4"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="2"/>
       <c r="P4" s="15"/>
       <c r="Q4" s="4"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R4" s="15"/>
+      <c r="S4" s="4"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>28</v>
       </c>
@@ -1619,20 +1663,22 @@
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
       <c r="H5" s="5"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="7"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="5"/>
       <c r="P5" s="16"/>
       <c r="Q5" s="7"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R5" s="16"/>
+      <c r="S5" s="7"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>25</v>
       </c>
@@ -1644,20 +1690,22 @@
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
       <c r="H6" s="5"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="7"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="5"/>
       <c r="P6" s="16"/>
       <c r="Q6" s="7"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R6" s="16"/>
+      <c r="S6" s="7"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="39" t="s">
         <v>155</v>
       </c>
@@ -1669,20 +1717,22 @@
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
       <c r="H7" s="5"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="16"/>
-      <c r="O7" s="7"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="5"/>
       <c r="P7" s="16"/>
       <c r="Q7" s="7"/>
-    </row>
-    <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R7" s="16"/>
+      <c r="S7" s="7"/>
+    </row>
+    <row r="8" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>33</v>
       </c>
@@ -1694,759 +1744,791 @@
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
       <c r="H8" s="8"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="10"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="8"/>
       <c r="P8" s="17"/>
       <c r="Q8" s="10"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R8" s="17"/>
+      <c r="S8" s="10"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D9" s="1">
         <v>1</v>
       </c>
       <c r="E9" s="1">
         <v>2</v>
       </c>
-      <c r="F9" s="1">
+      <c r="H9" s="1">
         <v>3</v>
       </c>
-      <c r="G9" s="1">
+      <c r="I9" s="1">
         <v>4</v>
       </c>
-      <c r="H9" s="1">
+      <c r="J9" s="1">
         <v>5</v>
       </c>
-      <c r="I9" s="1">
+      <c r="K9" s="1">
         <v>6</v>
       </c>
-      <c r="J9" s="1">
+      <c r="L9" s="1">
         <v>7</v>
       </c>
-      <c r="K9" s="1">
+      <c r="M9" s="1">
         <v>8</v>
       </c>
-      <c r="L9" s="1">
+      <c r="N9" s="1">
         <v>9</v>
       </c>
-      <c r="M9" s="1">
+      <c r="O9" s="1">
         <v>10</v>
       </c>
-      <c r="N9" s="1">
+      <c r="P9" s="1">
         <v>11</v>
       </c>
-      <c r="O9" s="1">
+      <c r="Q9" s="1">
         <v>12</v>
       </c>
-      <c r="P9" s="1">
+      <c r="R9" s="1">
         <v>13</v>
       </c>
-      <c r="Q9" s="1">
+      <c r="S9" s="1">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="M13" s="22" t="s">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="73" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="72" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" s="73" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="72" t="s">
+        <v>194</v>
+      </c>
+      <c r="O13" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="P13" s="22" t="s">
+      <c r="R13" s="22" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="M14" s="40" t="s">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="73" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="72" t="s">
+        <v>191</v>
+      </c>
+      <c r="O14" s="40" t="s">
         <v>138</v>
       </c>
-      <c r="P14" s="40" t="s">
+      <c r="R14" s="40" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="M15" s="30" t="s">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="73" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" s="72" t="s">
+        <v>192</v>
+      </c>
+      <c r="O15" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="P15" s="30" t="s">
+      <c r="R15" s="30" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="M16" s="30" t="s">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O16" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="P16" s="30" t="s">
+      <c r="R16" s="30" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="17" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D17" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="E17" s="65" t="s">
+      <c r="E17" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="F17" s="66"/>
-      <c r="G17" s="66"/>
-      <c r="H17" s="66"/>
-      <c r="I17" s="66"/>
-      <c r="J17" s="27" t="s">
+      <c r="F17" s="51"/>
+      <c r="G17" s="51"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="51"/>
+      <c r="K17" s="51"/>
+      <c r="L17" s="27" t="s">
         <v>153</v>
       </c>
-      <c r="K17" s="43" t="s">
+      <c r="M17" s="43" t="s">
         <v>145</v>
       </c>
-      <c r="L17" s="30" t="s">
+      <c r="N17" s="30" t="s">
         <v>144</v>
       </c>
-      <c r="M17" s="1" t="s">
+      <c r="O17" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="N17" s="30" t="s">
+      <c r="P17" s="30" t="s">
         <v>142</v>
       </c>
-      <c r="O17" s="30" t="s">
+      <c r="Q17" s="30" t="s">
         <v>143</v>
       </c>
-      <c r="P17" s="22" t="s">
+      <c r="R17" s="22" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="18" spans="4:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D18" s="58" t="s">
+    <row r="18" spans="4:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="66" t="s">
         <v>176</v>
       </c>
-      <c r="J18" s="33" t="s">
+      <c r="L18" s="33" t="s">
         <v>125</v>
       </c>
-      <c r="M18" s="30" t="s">
+      <c r="O18" s="30" t="s">
         <v>131</v>
       </c>
-      <c r="P18" s="30" t="s">
+      <c r="R18" s="30" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="19" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="D19" s="59"/>
-      <c r="G19" s="22" t="s">
+    <row r="19" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D19" s="67"/>
+      <c r="I19" s="22" t="s">
         <v>166</v>
       </c>
-      <c r="J19" s="44" t="s">
+      <c r="L19" s="44" t="s">
         <v>179</v>
       </c>
-      <c r="M19" s="30" t="s">
+      <c r="O19" s="30" t="s">
         <v>130</v>
       </c>
-      <c r="P19" s="30" t="s">
+      <c r="R19" s="30" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="20" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="D20" s="59"/>
-      <c r="G20" s="41" t="s">
+    <row r="20" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D20" s="67"/>
+      <c r="I20" s="41" t="s">
         <v>169</v>
       </c>
-      <c r="J20" s="29" t="s">
+      <c r="L20" s="29" t="s">
         <v>177</v>
       </c>
-      <c r="M20" s="22" t="s">
+      <c r="O20" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="N20" s="30" t="s">
+      <c r="P20" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="O20" s="40" t="s">
+      <c r="Q20" s="40" t="s">
         <v>134</v>
       </c>
-      <c r="P20" s="22" t="s">
+      <c r="R20" s="22" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="21" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="D21" s="60"/>
-      <c r="G21" s="29" t="s">
+    <row r="21" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D21" s="68"/>
+      <c r="I21" s="29" t="s">
         <v>168</v>
       </c>
-      <c r="J21" s="29" t="s">
+      <c r="L21" s="29" t="s">
         <v>170</v>
       </c>
-      <c r="M21" s="30" t="s">
+      <c r="O21" s="30" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="22" spans="4:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D22" s="22" t="s">
         <v>172</v>
       </c>
       <c r="E22" s="29" t="s">
         <v>175</v>
       </c>
-      <c r="F22" s="29" t="s">
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29" t="s">
         <v>174</v>
       </c>
-      <c r="G22" s="22" t="s">
+      <c r="I22" s="22" t="s">
         <v>164</v>
       </c>
-      <c r="H22" s="29" t="s">
+      <c r="J22" s="29" t="s">
         <v>181</v>
       </c>
-      <c r="I22" s="29" t="s">
+      <c r="K22" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="J22" s="22" t="s">
+      <c r="L22" s="22" t="s">
         <v>171</v>
       </c>
-      <c r="M22" s="30" t="s">
+      <c r="O22" s="30" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="23" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="G23" s="41" t="s">
+    <row r="23" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="I23" s="41" t="s">
         <v>163</v>
       </c>
-      <c r="J23" s="42" t="s">
+      <c r="L23" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="M23" s="30" t="s">
+      <c r="O23" s="30" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="24" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="G24" s="29" t="s">
+    <row r="24" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="I24" s="29" t="s">
         <v>162</v>
       </c>
-      <c r="J24" s="22" t="s">
+      <c r="L24" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="K24" s="24" t="s">
+      <c r="M24" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="L24" s="24" t="s">
+      <c r="N24" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="M24" s="22" t="s">
+      <c r="O24" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="N24" s="25" t="s">
+      <c r="P24" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="O24" s="25" t="s">
+      <c r="Q24" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="P24" s="22" t="s">
+      <c r="R24" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="T24" s="22" t="s">
+      <c r="V24" s="22" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="25" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="G25" s="22" t="s">
+    <row r="25" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="I25" s="22" t="s">
         <v>161</v>
       </c>
-      <c r="J25" s="23" t="s">
+      <c r="L25" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="M25" s="23" t="s">
+      <c r="O25" s="71" t="s">
         <v>56</v>
       </c>
-      <c r="P25" s="25" t="s">
+      <c r="R25" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="T25" s="28" t="s">
+      <c r="V25" s="28" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="26" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="G26" s="29" t="s">
+    <row r="26" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="I26" s="29" t="s">
         <v>160</v>
       </c>
-      <c r="J26" s="24" t="s">
+      <c r="L26" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="M26" s="24" t="s">
+      <c r="O26" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="P26" s="25" t="s">
+      <c r="R26" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="T26" s="38" t="s">
+      <c r="V26" s="38" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="G27" s="29" t="s">
+    <row r="27" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="I27" s="29" t="s">
         <v>159</v>
       </c>
-      <c r="J27" s="24" t="s">
+      <c r="L27" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="M27" s="24" t="s">
+      <c r="O27" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="P27" s="22" t="s">
+      <c r="R27" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="Q27" s="25" t="s">
+      <c r="S27" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="R27" s="25" t="s">
+      <c r="T27" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="S27" s="37" t="s">
+      <c r="U27" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="T27" s="27" t="s">
+      <c r="V27" s="27" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="G28" s="22" t="s">
+    <row r="28" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="I28" s="22" t="s">
         <v>158</v>
       </c>
-      <c r="H28" s="29" t="s">
+      <c r="J28" s="29" t="s">
         <v>157</v>
       </c>
-      <c r="I28" s="29" t="s">
+      <c r="K28" s="29" t="s">
         <v>156</v>
       </c>
-      <c r="J28" s="22" t="s">
+      <c r="L28" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="K28" s="24" t="s">
+      <c r="M28" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="L28" s="24" t="s">
+      <c r="N28" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="M28" s="22" t="s">
+      <c r="O28" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="P28" s="25" t="s">
+      <c r="R28" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="T28" s="33" t="s">
+      <c r="V28" s="33" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="29" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="G29" s="29" t="s">
+    <row r="29" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="I29" s="29" t="s">
         <v>180</v>
       </c>
-      <c r="J29" s="23" t="s">
+      <c r="L29" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="M29" s="23" t="s">
+      <c r="O29" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="P29" s="25" t="s">
+      <c r="R29" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="T29" s="64" t="s">
+      <c r="V29" s="47" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="30" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="G30" s="41" t="s">
+    <row r="30" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="I30" s="41" t="s">
         <v>184</v>
       </c>
-      <c r="J30" s="24" t="s">
+      <c r="L30" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="M30" s="24" t="s">
+      <c r="O30" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="P30" s="25" t="s">
+      <c r="R30" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="T30" s="62"/>
-    </row>
-    <row r="31" spans="4:20" x14ac:dyDescent="0.25">
-      <c r="G31" s="22" t="s">
+      <c r="V30" s="48"/>
+    </row>
+    <row r="31" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="I31" s="22" t="s">
         <v>173</v>
       </c>
-      <c r="J31" s="22" t="s">
+      <c r="L31" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="K31" s="24" t="s">
+      <c r="M31" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="L31" s="24" t="s">
+      <c r="N31" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="M31" s="22" t="s">
+      <c r="O31" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="N31" s="25" t="s">
+      <c r="P31" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="O31" s="25" t="s">
+      <c r="Q31" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="P31" s="22" t="s">
+      <c r="R31" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="T31" s="62"/>
-    </row>
-    <row r="32" spans="4:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G32" s="61" t="s">
+      <c r="V31" s="48"/>
+    </row>
+    <row r="32" spans="4:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I32" s="69" t="s">
         <v>167</v>
       </c>
-      <c r="J32" s="24" t="s">
+      <c r="L32" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="P32" s="25" t="s">
+      <c r="R32" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="T32" s="62"/>
-    </row>
-    <row r="33" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="G33" s="62"/>
-      <c r="J33" s="32" t="s">
+      <c r="V32" s="48"/>
+    </row>
+    <row r="33" spans="9:22" x14ac:dyDescent="0.25">
+      <c r="I33" s="48"/>
+      <c r="L33" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="P33" s="25" t="s">
+      <c r="R33" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="T33" s="62"/>
-    </row>
-    <row r="34" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="G34" s="62"/>
-      <c r="J34" s="27" t="s">
+      <c r="V33" s="48"/>
+    </row>
+    <row r="34" spans="9:22" x14ac:dyDescent="0.25">
+      <c r="I34" s="48"/>
+      <c r="L34" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="P34" s="28" t="s">
+      <c r="R34" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="T34" s="62"/>
-    </row>
-    <row r="35" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="G35" s="62"/>
-      <c r="J35" s="33" t="s">
+      <c r="V34" s="48"/>
+    </row>
+    <row r="35" spans="9:22" x14ac:dyDescent="0.25">
+      <c r="I35" s="48"/>
+      <c r="L35" s="33" t="s">
         <v>124</v>
       </c>
-      <c r="K35" s="31" t="s">
+      <c r="M35" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="L35" s="22" t="s">
+      <c r="N35" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="M35" s="28" t="s">
+      <c r="O35" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="N35" s="25" t="s">
+      <c r="P35" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="O35" s="25" t="s">
+      <c r="Q35" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="P35" s="22" t="s">
+      <c r="R35" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="T35" s="62"/>
-    </row>
-    <row r="36" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="G36" s="62"/>
-      <c r="J36" s="24" t="s">
+      <c r="V35" s="48"/>
+    </row>
+    <row r="36" spans="9:22" x14ac:dyDescent="0.25">
+      <c r="I36" s="48"/>
+      <c r="L36" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="L36" s="31" t="s">
+      <c r="N36" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="T36" s="62"/>
-    </row>
-    <row r="37" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="G37" s="62"/>
-      <c r="J37" s="24" t="s">
+      <c r="V36" s="48"/>
+    </row>
+    <row r="37" spans="9:22" x14ac:dyDescent="0.25">
+      <c r="I37" s="48"/>
+      <c r="L37" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="L37" s="31" t="s">
+      <c r="N37" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="T37" s="62"/>
-    </row>
-    <row r="38" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="G38" s="63"/>
-      <c r="J38" s="24" t="s">
+      <c r="V37" s="48"/>
+    </row>
+    <row r="38" spans="9:22" x14ac:dyDescent="0.25">
+      <c r="I38" s="49"/>
+      <c r="L38" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="L38" s="31" t="s">
+      <c r="N38" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="T38" s="62"/>
-    </row>
-    <row r="39" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="G39" s="22" t="s">
+      <c r="V38" s="48"/>
+    </row>
+    <row r="39" spans="9:22" x14ac:dyDescent="0.25">
+      <c r="I39" s="22" t="s">
         <v>173</v>
       </c>
-      <c r="H39" s="29" t="s">
+      <c r="J39" s="29" t="s">
         <v>182</v>
       </c>
-      <c r="I39" s="41" t="s">
+      <c r="K39" s="41" t="s">
         <v>178</v>
       </c>
-      <c r="J39" s="22" t="s">
+      <c r="L39" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="L39" s="22" t="s">
+      <c r="N39" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="M39" s="31" t="s">
+      <c r="O39" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="N39" s="31" t="s">
+      <c r="P39" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="O39" s="36" t="s">
+      <c r="Q39" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="P39" s="22" t="s">
+      <c r="R39" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="T39" s="62"/>
-    </row>
-    <row r="40" spans="7:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J40" s="67" t="s">
+      <c r="V39" s="48"/>
+    </row>
+    <row r="40" spans="9:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L40" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="L40" s="31" t="s">
+      <c r="N40" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="T40" s="62"/>
-    </row>
-    <row r="41" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="J41" s="68"/>
-      <c r="L41" s="31" t="s">
+      <c r="V40" s="48"/>
+    </row>
+    <row r="41" spans="9:22" x14ac:dyDescent="0.25">
+      <c r="L41" s="53"/>
+      <c r="N41" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="T41" s="62"/>
-    </row>
-    <row r="42" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="J42" s="68"/>
-      <c r="L42" s="36" t="s">
+      <c r="V41" s="48"/>
+    </row>
+    <row r="42" spans="9:22" x14ac:dyDescent="0.25">
+      <c r="L42" s="53"/>
+      <c r="N42" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="T42" s="63"/>
-    </row>
-    <row r="43" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="J43" s="68"/>
-      <c r="L43" s="22" t="s">
+      <c r="V42" s="49"/>
+    </row>
+    <row r="43" spans="9:22" x14ac:dyDescent="0.25">
+      <c r="L43" s="53"/>
+      <c r="N43" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="M43" s="31" t="s">
+      <c r="O43" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="N43" s="31" t="s">
+      <c r="P43" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="O43" s="22" t="s">
+      <c r="Q43" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="P43" s="31" t="s">
+      <c r="R43" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="Q43" s="31" t="s">
+      <c r="S43" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="R43" s="36" t="s">
+      <c r="T43" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="S43" s="35" t="s">
+      <c r="U43" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="T43" s="42" t="s">
+      <c r="V43" s="42" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="44" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="J44" s="68"/>
-      <c r="O44" s="31" t="s">
+    <row r="44" spans="9:22" x14ac:dyDescent="0.25">
+      <c r="L44" s="53"/>
+      <c r="Q44" s="31" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="45" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="J45" s="68"/>
-      <c r="O45" s="31" t="s">
+    <row r="45" spans="9:22" x14ac:dyDescent="0.25">
+      <c r="L45" s="53"/>
+      <c r="Q45" s="31" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="46" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="J46" s="69"/>
-      <c r="O46" s="36" t="s">
+    <row r="46" spans="9:22" x14ac:dyDescent="0.25">
+      <c r="L46" s="54"/>
+      <c r="Q46" s="36" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="47" spans="7:20" x14ac:dyDescent="0.25">
-      <c r="J47" s="22" t="s">
+    <row r="47" spans="9:22" x14ac:dyDescent="0.25">
+      <c r="L47" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="K47" s="47" t="s">
+      <c r="M47" s="55" t="s">
         <v>111</v>
       </c>
-      <c r="L47" s="48"/>
-      <c r="M47" s="48"/>
-      <c r="N47" s="49"/>
-      <c r="O47" s="22" t="s">
+      <c r="N47" s="56"/>
+      <c r="O47" s="56"/>
+      <c r="P47" s="57"/>
+      <c r="Q47" s="22" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="J50" s="26" t="s">
+    <row r="50" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="L50" s="26" t="s">
         <v>186</v>
       </c>
-      <c r="K50" s="22" t="s">
+      <c r="M50" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="L50" s="22" t="s">
+      <c r="N50" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="M50" s="34" t="s">
+      <c r="O50" s="34" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="51" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I51" s="24" t="s">
+    <row r="51" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K51" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="J51" s="24">
+      <c r="L51" s="24">
         <v>21</v>
       </c>
-      <c r="K51" s="24">
+      <c r="M51" s="24">
         <v>15</v>
       </c>
-      <c r="L51" s="24">
+      <c r="N51" s="24">
         <v>6</v>
       </c>
-      <c r="M51" s="24">
+      <c r="O51" s="24">
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I52" s="25" t="s">
+    <row r="52" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K52" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="J52" s="25">
+      <c r="L52" s="25">
         <v>21</v>
       </c>
-      <c r="K52" s="25">
+      <c r="M52" s="25">
         <v>11</v>
       </c>
-      <c r="L52" s="25">
+      <c r="N52" s="25">
         <v>10</v>
       </c>
-      <c r="M52" s="25">
+      <c r="O52" s="25">
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I53" s="31" t="s">
+    <row r="53" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K53" s="31" t="s">
         <v>119</v>
       </c>
-      <c r="J53" s="31">
+      <c r="L53" s="31">
         <v>22</v>
       </c>
-      <c r="K53" s="31">
+      <c r="M53" s="31">
         <v>10</v>
       </c>
-      <c r="L53" s="31">
+      <c r="N53" s="31">
         <v>12</v>
       </c>
-      <c r="M53" s="31">
+      <c r="O53" s="31">
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I54" s="30" t="s">
+    <row r="54" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K54" s="30" t="s">
         <v>154</v>
       </c>
-      <c r="J54" s="30">
+      <c r="L54" s="30">
         <v>20</v>
       </c>
-      <c r="K54" s="30">
+      <c r="M54" s="30">
         <v>13</v>
       </c>
-      <c r="L54" s="30">
+      <c r="N54" s="30">
         <v>7</v>
       </c>
-      <c r="M54" s="30">
+      <c r="O54" s="30">
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I55" s="29" t="s">
+    <row r="55" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K55" s="29" t="s">
         <v>155</v>
       </c>
-      <c r="J55" s="29">
+      <c r="L55" s="29">
         <v>20</v>
       </c>
-      <c r="K55" s="29">
+      <c r="M55" s="29">
         <v>12</v>
       </c>
-      <c r="L55" s="29">
+      <c r="N55" s="29">
         <v>8</v>
       </c>
-      <c r="M55" s="29">
+      <c r="O55" s="29">
         <v>8</v>
       </c>
     </row>
-    <row r="56" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I56" s="42" t="s">
+    <row r="56" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K56" s="42" t="s">
         <v>185</v>
-      </c>
-      <c r="J56" s="42">
-        <v>0</v>
-      </c>
-      <c r="K56" s="42">
-        <v>0</v>
       </c>
       <c r="L56" s="42">
         <v>0</v>
       </c>
       <c r="M56" s="42">
+        <v>0</v>
+      </c>
+      <c r="N56" s="42">
+        <v>0</v>
+      </c>
+      <c r="O56" s="42">
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="9:13" x14ac:dyDescent="0.25">
-      <c r="I57" s="45" t="s">
+    <row r="57" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K57" s="45" t="s">
         <v>187</v>
-      </c>
-      <c r="J57" s="46">
-        <f>SUM(J51:J56)</f>
-        <v>104</v>
-      </c>
-      <c r="K57" s="46">
-        <f>SUM(K51:K56)</f>
-        <v>61</v>
       </c>
       <c r="L57" s="46">
         <f>SUM(L51:L56)</f>
-        <v>43</v>
+        <v>104</v>
       </c>
       <c r="M57" s="46">
         <f>SUM(M51:M56)</f>
+        <v>61</v>
+      </c>
+      <c r="N57" s="46">
+        <f>SUM(N51:N56)</f>
+        <v>43</v>
+      </c>
+      <c r="O57" s="46">
+        <f>SUM(O51:O56)</f>
         <v>40</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="T29:T42"/>
-    <mergeCell ref="E17:I17"/>
-    <mergeCell ref="J40:J46"/>
-    <mergeCell ref="K47:N47"/>
-    <mergeCell ref="D1:Q1"/>
+    <mergeCell ref="V29:V42"/>
+    <mergeCell ref="E17:K17"/>
+    <mergeCell ref="L40:L46"/>
+    <mergeCell ref="M47:P47"/>
+    <mergeCell ref="D1:S1"/>
     <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:S3"/>
     <mergeCell ref="D18:D21"/>
-    <mergeCell ref="G32:G38"/>
+    <mergeCell ref="I32:I38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Integration of levels V1, V2, V3, V4, H1, H2 with prototype values
</commit_message>
<xml_diff>
--- a/Unstable/StarFighter/Documentation/Factions.xlsx
+++ b/Unstable/StarFighter/Documentation/Factions.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Vanguard" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="239">
   <si>
     <t>Faction</t>
   </si>
@@ -605,13 +605,145 @@
   </si>
   <si>
     <t>Commandante Astride (Chef de l'Avant-Garde)</t>
+  </si>
+  <si>
+    <t>V1</t>
+  </si>
+  <si>
+    <t>V2</t>
+  </si>
+  <si>
+    <t>V3</t>
+  </si>
+  <si>
+    <t>V4</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>V5</t>
+  </si>
+  <si>
+    <t>V6</t>
+  </si>
+  <si>
+    <t>V7</t>
+  </si>
+  <si>
+    <t>V8</t>
+  </si>
+  <si>
+    <t>V9</t>
+  </si>
+  <si>
+    <t>H3</t>
+  </si>
+  <si>
+    <t>H4</t>
+  </si>
+  <si>
+    <t>H5</t>
+  </si>
+  <si>
+    <t>H6</t>
+  </si>
+  <si>
+    <t>V10</t>
+  </si>
+  <si>
+    <t>V11</t>
+  </si>
+  <si>
+    <t>V12</t>
+  </si>
+  <si>
+    <t>alpha1</t>
+  </si>
+  <si>
+    <t>sigma1</t>
+  </si>
+  <si>
+    <t>beta1</t>
+  </si>
+  <si>
+    <t>gamma1</t>
+  </si>
+  <si>
+    <t>alpha3</t>
+  </si>
+  <si>
+    <t>sigma2 / sigma3</t>
+  </si>
+  <si>
+    <t>beta1 / beta2</t>
+  </si>
+  <si>
+    <t>gamma2</t>
+  </si>
+  <si>
+    <t>beta2 / beta3</t>
+  </si>
+  <si>
+    <t>alpha2 / alpha3</t>
+  </si>
+  <si>
+    <t>delta1</t>
+  </si>
+  <si>
+    <t>gamma1 / gamma2</t>
+  </si>
+  <si>
+    <t>delta2</t>
+  </si>
+  <si>
+    <t>alpha3 / sigma3</t>
+  </si>
+  <si>
+    <t>beta1/ beta 2/ beta3</t>
+  </si>
+  <si>
+    <t>gamma3</t>
+  </si>
+  <si>
+    <t>sigma2/sigma3</t>
+  </si>
+  <si>
+    <t>delta3</t>
+  </si>
+  <si>
+    <t>gamma1 / gamma2 / gamma3</t>
+  </si>
+  <si>
+    <t>delta2/delta3</t>
+  </si>
+  <si>
+    <t>delta1/delta2</t>
+  </si>
+  <si>
+    <t>alpha2 / sigma2</t>
+  </si>
+  <si>
+    <t>beta 2/ beta3</t>
+  </si>
+  <si>
+    <t>beta2</t>
+  </si>
+  <si>
+    <t>sigma1 / sigma 2</t>
+  </si>
+  <si>
+    <t>alpha1 / alpha 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -642,8 +774,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -692,8 +852,28 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -946,11 +1126,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1090,6 +1289,35 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="22" xfId="4"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="22" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1159,20 +1387,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Input" xfId="4" builtinId="20"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1480,8 +1700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24:O38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1517,24 +1737,24 @@
       <c r="C1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="58" t="s">
+      <c r="D1" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58"/>
-      <c r="P1" s="58"/>
-      <c r="Q1" s="58"/>
-      <c r="R1" s="58"/>
-      <c r="S1" s="59"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="73"/>
+      <c r="O1" s="73"/>
+      <c r="P1" s="73"/>
+      <c r="Q1" s="73"/>
+      <c r="R1" s="73"/>
+      <c r="S1" s="74"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
@@ -1593,36 +1813,36 @@
       <c r="A3" s="16"/>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
-      <c r="D3" s="60" t="s">
+      <c r="D3" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="61"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="62" t="s">
+      <c r="E3" s="76"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="77" t="s">
         <v>36</v>
       </c>
-      <c r="I3" s="61"/>
-      <c r="J3" s="62" t="s">
+      <c r="I3" s="76"/>
+      <c r="J3" s="77" t="s">
         <v>188</v>
       </c>
-      <c r="K3" s="61"/>
-      <c r="L3" s="63" t="s">
+      <c r="K3" s="76"/>
+      <c r="L3" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="M3" s="64"/>
-      <c r="N3" s="63" t="s">
+      <c r="M3" s="79"/>
+      <c r="N3" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="65"/>
-      <c r="P3" s="63" t="s">
+      <c r="O3" s="80"/>
+      <c r="P3" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="Q3" s="64"/>
-      <c r="R3" s="62" t="s">
+      <c r="Q3" s="79"/>
+      <c r="R3" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="S3" s="61"/>
+      <c r="S3" s="76"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
@@ -1804,18 +2024,18 @@
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="73" t="s">
+      <c r="A12" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="72" t="s">
+      <c r="B12" s="49" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="73" t="s">
+      <c r="A13" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="B13" s="72" t="s">
+      <c r="B13" s="49" t="s">
         <v>194</v>
       </c>
       <c r="O13" s="22" t="s">
@@ -1826,10 +2046,10 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="73" t="s">
+      <c r="A14" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="72" t="s">
+      <c r="B14" s="49" t="s">
         <v>191</v>
       </c>
       <c r="O14" s="40" t="s">
@@ -1840,10 +2060,10 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="73" t="s">
+      <c r="A15" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="B15" s="72" t="s">
+      <c r="B15" s="49" t="s">
         <v>192</v>
       </c>
       <c r="O15" s="30" t="s">
@@ -1865,15 +2085,15 @@
       <c r="D17" s="22" t="s">
         <v>153</v>
       </c>
-      <c r="E17" s="50" t="s">
+      <c r="E17" s="65" t="s">
         <v>146</v>
       </c>
-      <c r="F17" s="51"/>
-      <c r="G17" s="51"/>
-      <c r="H17" s="51"/>
-      <c r="I17" s="51"/>
-      <c r="J17" s="51"/>
-      <c r="K17" s="51"/>
+      <c r="F17" s="66"/>
+      <c r="G17" s="66"/>
+      <c r="H17" s="66"/>
+      <c r="I17" s="66"/>
+      <c r="J17" s="66"/>
+      <c r="K17" s="66"/>
       <c r="L17" s="27" t="s">
         <v>153</v>
       </c>
@@ -1897,7 +2117,7 @@
       </c>
     </row>
     <row r="18" spans="4:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D18" s="66" t="s">
+      <c r="D18" s="81" t="s">
         <v>176</v>
       </c>
       <c r="L18" s="33" t="s">
@@ -1911,7 +2131,7 @@
       </c>
     </row>
     <row r="19" spans="4:22" x14ac:dyDescent="0.25">
-      <c r="D19" s="67"/>
+      <c r="D19" s="82"/>
       <c r="I19" s="22" t="s">
         <v>166</v>
       </c>
@@ -1926,7 +2146,7 @@
       </c>
     </row>
     <row r="20" spans="4:22" x14ac:dyDescent="0.25">
-      <c r="D20" s="67"/>
+      <c r="D20" s="82"/>
       <c r="I20" s="41" t="s">
         <v>169</v>
       </c>
@@ -1947,7 +2167,7 @@
       </c>
     </row>
     <row r="21" spans="4:22" x14ac:dyDescent="0.25">
-      <c r="D21" s="68"/>
+      <c r="D21" s="83"/>
       <c r="I21" s="29" t="s">
         <v>168</v>
       </c>
@@ -2033,7 +2253,7 @@
       <c r="L25" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="O25" s="71" t="s">
+      <c r="O25" s="48" t="s">
         <v>56</v>
       </c>
       <c r="R25" s="25" t="s">
@@ -2128,7 +2348,7 @@
       <c r="R29" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="V29" s="47" t="s">
+      <c r="V29" s="62" t="s">
         <v>147</v>
       </c>
     </row>
@@ -2145,7 +2365,7 @@
       <c r="R30" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="V30" s="48"/>
+      <c r="V30" s="63"/>
     </row>
     <row r="31" spans="4:22" x14ac:dyDescent="0.25">
       <c r="I31" s="22" t="s">
@@ -2172,10 +2392,10 @@
       <c r="R31" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="V31" s="48"/>
+      <c r="V31" s="63"/>
     </row>
     <row r="32" spans="4:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I32" s="69" t="s">
+      <c r="I32" s="84" t="s">
         <v>167</v>
       </c>
       <c r="L32" s="24" t="s">
@@ -2184,30 +2404,30 @@
       <c r="R32" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="V32" s="48"/>
+      <c r="V32" s="63"/>
     </row>
     <row r="33" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I33" s="48"/>
+      <c r="I33" s="63"/>
       <c r="L33" s="32" t="s">
         <v>45</v>
       </c>
       <c r="R33" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="V33" s="48"/>
+      <c r="V33" s="63"/>
     </row>
     <row r="34" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I34" s="48"/>
+      <c r="I34" s="63"/>
       <c r="L34" s="27" t="s">
         <v>46</v>
       </c>
       <c r="R34" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="V34" s="48"/>
+      <c r="V34" s="63"/>
     </row>
     <row r="35" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I35" s="48"/>
+      <c r="I35" s="63"/>
       <c r="L35" s="33" t="s">
         <v>124</v>
       </c>
@@ -2229,37 +2449,37 @@
       <c r="R35" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="V35" s="48"/>
+      <c r="V35" s="63"/>
     </row>
     <row r="36" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I36" s="48"/>
+      <c r="I36" s="63"/>
       <c r="L36" s="24" t="s">
         <v>123</v>
       </c>
       <c r="N36" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="V36" s="48"/>
+      <c r="V36" s="63"/>
     </row>
     <row r="37" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I37" s="48"/>
+      <c r="I37" s="63"/>
       <c r="L37" s="24" t="s">
         <v>122</v>
       </c>
       <c r="N37" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="V37" s="48"/>
+      <c r="V37" s="63"/>
     </row>
     <row r="38" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="I38" s="49"/>
+      <c r="I38" s="64"/>
       <c r="L38" s="24" t="s">
         <v>121</v>
       </c>
       <c r="N38" s="31" t="s">
         <v>93</v>
       </c>
-      <c r="V38" s="48"/>
+      <c r="V38" s="63"/>
     </row>
     <row r="39" spans="9:22" x14ac:dyDescent="0.25">
       <c r="I39" s="22" t="s">
@@ -2289,33 +2509,33 @@
       <c r="R39" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="V39" s="48"/>
+      <c r="V39" s="63"/>
     </row>
     <row r="40" spans="9:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L40" s="52" t="s">
+      <c r="L40" s="67" t="s">
         <v>112</v>
       </c>
       <c r="N40" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="V40" s="48"/>
+      <c r="V40" s="63"/>
     </row>
     <row r="41" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="L41" s="53"/>
+      <c r="L41" s="68"/>
       <c r="N41" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="V41" s="48"/>
+      <c r="V41" s="63"/>
     </row>
     <row r="42" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="L42" s="53"/>
+      <c r="L42" s="68"/>
       <c r="N42" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="V42" s="49"/>
+      <c r="V42" s="64"/>
     </row>
     <row r="43" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="L43" s="53"/>
+      <c r="L43" s="68"/>
       <c r="N43" s="22" t="s">
         <v>101</v>
       </c>
@@ -2345,19 +2565,19 @@
       </c>
     </row>
     <row r="44" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="L44" s="53"/>
+      <c r="L44" s="68"/>
       <c r="Q44" s="31" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="45" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="L45" s="53"/>
+      <c r="L45" s="68"/>
       <c r="Q45" s="31" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="46" spans="9:22" x14ac:dyDescent="0.25">
-      <c r="L46" s="54"/>
+      <c r="L46" s="69"/>
       <c r="Q46" s="36" t="s">
         <v>107</v>
       </c>
@@ -2366,12 +2586,12 @@
       <c r="L47" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="M47" s="55" t="s">
+      <c r="M47" s="70" t="s">
         <v>111</v>
       </c>
-      <c r="N47" s="56"/>
-      <c r="O47" s="56"/>
-      <c r="P47" s="57"/>
+      <c r="N47" s="71"/>
+      <c r="O47" s="71"/>
+      <c r="P47" s="72"/>
       <c r="Q47" s="22" t="s">
         <v>108</v>
       </c>
@@ -2537,13 +2757,486 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="48" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="51"/>
+      <c r="B12" s="52"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="53"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="52"/>
+      <c r="B13" s="52"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="52"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="52"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="52"/>
+      <c r="B15" s="52"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="54"/>
+      <c r="B16" s="54"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="54"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="54"/>
+      <c r="B17" s="54"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="54"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="55" t="s">
+        <v>195</v>
+      </c>
+      <c r="B18" t="s">
+        <v>213</v>
+      </c>
+      <c r="C18" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="55" t="s">
+        <v>196</v>
+      </c>
+      <c r="B19" t="s">
+        <v>213</v>
+      </c>
+      <c r="C19" t="s">
+        <v>214</v>
+      </c>
+      <c r="D19" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="56" t="s">
+        <v>197</v>
+      </c>
+      <c r="B21" t="s">
+        <v>238</v>
+      </c>
+      <c r="C21" t="s">
+        <v>237</v>
+      </c>
+      <c r="D21" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="59" t="s">
+        <v>198</v>
+      </c>
+      <c r="B22" t="s">
+        <v>238</v>
+      </c>
+      <c r="C22" t="s">
+        <v>237</v>
+      </c>
+      <c r="D22" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="56" t="s">
+        <v>199</v>
+      </c>
+      <c r="B24" t="s">
+        <v>238</v>
+      </c>
+      <c r="C24" t="s">
+        <v>237</v>
+      </c>
+      <c r="D24" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="56" t="s">
+        <v>200</v>
+      </c>
+      <c r="B25" t="s">
+        <v>238</v>
+      </c>
+      <c r="C25" t="s">
+        <v>237</v>
+      </c>
+      <c r="D25" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="57" t="s">
+        <v>201</v>
+      </c>
+      <c r="B27" t="s">
+        <v>217</v>
+      </c>
+      <c r="C27" t="s">
+        <v>218</v>
+      </c>
+      <c r="D27" t="s">
+        <v>219</v>
+      </c>
+      <c r="E27" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="57" t="s">
+        <v>202</v>
+      </c>
+      <c r="B28" t="s">
+        <v>222</v>
+      </c>
+      <c r="C28" t="s">
+        <v>218</v>
+      </c>
+      <c r="D28" t="s">
+        <v>221</v>
+      </c>
+      <c r="E28" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="60" t="s">
+        <v>203</v>
+      </c>
+      <c r="B29" t="s">
+        <v>222</v>
+      </c>
+      <c r="C29" t="s">
+        <v>224</v>
+      </c>
+      <c r="D29" t="s">
+        <v>221</v>
+      </c>
+      <c r="E29" t="s">
+        <v>218</v>
+      </c>
+      <c r="F29" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="57" t="s">
+        <v>204</v>
+      </c>
+      <c r="B31" t="s">
+        <v>222</v>
+      </c>
+      <c r="C31" t="s">
+        <v>218</v>
+      </c>
+      <c r="D31" t="s">
+        <v>221</v>
+      </c>
+      <c r="E31" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="60" t="s">
+        <v>205</v>
+      </c>
+      <c r="B32" t="s">
+        <v>222</v>
+      </c>
+      <c r="C32" t="s">
+        <v>224</v>
+      </c>
+      <c r="D32" t="s">
+        <v>221</v>
+      </c>
+      <c r="E32" t="s">
+        <v>218</v>
+      </c>
+      <c r="F32" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="57" t="s">
+        <v>206</v>
+      </c>
+      <c r="B34" t="s">
+        <v>222</v>
+      </c>
+      <c r="C34" t="s">
+        <v>218</v>
+      </c>
+      <c r="D34" t="s">
+        <v>221</v>
+      </c>
+      <c r="E34" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="57" t="s">
+        <v>207</v>
+      </c>
+      <c r="B35" t="s">
+        <v>222</v>
+      </c>
+      <c r="C35" t="s">
+        <v>224</v>
+      </c>
+      <c r="D35" t="s">
+        <v>221</v>
+      </c>
+      <c r="E35" t="s">
+        <v>218</v>
+      </c>
+      <c r="F35" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="58" t="s">
+        <v>208</v>
+      </c>
+      <c r="B37" t="s">
+        <v>226</v>
+      </c>
+      <c r="C37" t="s">
+        <v>227</v>
+      </c>
+      <c r="D37" t="s">
+        <v>229</v>
+      </c>
+      <c r="E37" t="s">
+        <v>228</v>
+      </c>
+      <c r="F37" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="61" t="s">
+        <v>209</v>
+      </c>
+      <c r="B38" t="s">
+        <v>226</v>
+      </c>
+      <c r="C38" t="s">
+        <v>227</v>
+      </c>
+      <c r="D38" t="s">
+        <v>229</v>
+      </c>
+      <c r="E38" t="s">
+        <v>231</v>
+      </c>
+      <c r="F38" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="58" t="s">
+        <v>210</v>
+      </c>
+      <c r="B40" t="s">
+        <v>234</v>
+      </c>
+      <c r="C40" t="s">
+        <v>221</v>
+      </c>
+      <c r="D40" t="s">
+        <v>229</v>
+      </c>
+      <c r="E40" t="s">
+        <v>228</v>
+      </c>
+      <c r="F40" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="58" t="s">
+        <v>211</v>
+      </c>
+      <c r="B41" t="s">
+        <v>226</v>
+      </c>
+      <c r="C41" t="s">
+        <v>227</v>
+      </c>
+      <c r="D41" t="s">
+        <v>229</v>
+      </c>
+      <c r="E41" t="s">
+        <v>231</v>
+      </c>
+      <c r="F41" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="58" t="s">
+        <v>212</v>
+      </c>
+      <c r="B42" t="s">
+        <v>226</v>
+      </c>
+      <c r="C42" t="s">
+        <v>235</v>
+      </c>
+      <c r="D42" t="s">
+        <v>229</v>
+      </c>
+      <c r="E42" t="s">
+        <v>231</v>
+      </c>
+      <c r="F42" t="s">
+        <v>232</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
All Vanguard scenes integration
</commit_message>
<xml_diff>
--- a/Unstable/StarFighter/Documentation/Factions.xlsx
+++ b/Unstable/StarFighter/Documentation/Factions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="240">
   <si>
     <t>Faction</t>
   </si>
@@ -709,9 +709,6 @@
     <t>gamma3</t>
   </si>
   <si>
-    <t>sigma2/sigma3</t>
-  </si>
-  <si>
     <t>delta3</t>
   </si>
   <si>
@@ -724,9 +721,6 @@
     <t>delta1/delta2</t>
   </si>
   <si>
-    <t>alpha2 / sigma2</t>
-  </si>
-  <si>
     <t>beta 2/ beta3</t>
   </si>
   <si>
@@ -737,6 +731,15 @@
   </si>
   <si>
     <t>alpha1 / alpha 2</t>
+  </si>
+  <si>
+    <t>zeta</t>
+  </si>
+  <si>
+    <t>sigma1 / sigma2</t>
+  </si>
+  <si>
+    <t>beta2 / beta3 / gamma1 / gamma2</t>
   </si>
 </sst>
 </file>
@@ -2757,10 +2760,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2768,7 +2771,7 @@
     <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -2955,10 +2958,10 @@
         <v>197</v>
       </c>
       <c r="B21" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C21" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D21" t="s">
         <v>215</v>
@@ -2969,10 +2972,10 @@
         <v>198</v>
       </c>
       <c r="B22" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C22" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D22" t="s">
         <v>216</v>
@@ -2983,13 +2986,16 @@
         <v>199</v>
       </c>
       <c r="B24" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C24" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D24" t="s">
         <v>216</v>
+      </c>
+      <c r="E24" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -2997,13 +3003,16 @@
         <v>200</v>
       </c>
       <c r="B25" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C25" t="s">
+        <v>235</v>
+      </c>
+      <c r="D25" t="s">
+        <v>234</v>
+      </c>
+      <c r="E25" t="s">
         <v>237</v>
-      </c>
-      <c r="D25" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -3011,10 +3020,10 @@
         <v>201</v>
       </c>
       <c r="B27" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="C27" t="s">
-        <v>218</v>
+        <v>238</v>
       </c>
       <c r="D27" t="s">
         <v>219</v>
@@ -3039,25 +3048,25 @@
       <c r="E28" t="s">
         <v>220</v>
       </c>
+      <c r="F28" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="60" t="s">
         <v>203</v>
       </c>
       <c r="B29" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="C29" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="D29" t="s">
-        <v>221</v>
+        <v>239</v>
       </c>
       <c r="E29" t="s">
-        <v>218</v>
-      </c>
-      <c r="F29" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -3071,7 +3080,7 @@
         <v>218</v>
       </c>
       <c r="D31" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E31" t="s">
         <v>224</v>
@@ -3085,19 +3094,19 @@
         <v>222</v>
       </c>
       <c r="C32" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="D32" t="s">
         <v>221</v>
       </c>
       <c r="E32" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="F32" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="57" t="s">
         <v>206</v>
       </c>
@@ -3114,7 +3123,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="57" t="s">
         <v>207</v>
       </c>
@@ -3134,7 +3143,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="58" t="s">
         <v>208</v>
       </c>
@@ -3145,16 +3154,13 @@
         <v>227</v>
       </c>
       <c r="D37" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E37" t="s">
-        <v>228</v>
-      </c>
-      <c r="F37" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="61" t="s">
         <v>209</v>
       </c>
@@ -3165,27 +3171,24 @@
         <v>227</v>
       </c>
       <c r="D38" t="s">
+        <v>230</v>
+      </c>
+      <c r="E38" t="s">
         <v>229</v>
       </c>
-      <c r="E38" t="s">
-        <v>231</v>
-      </c>
-      <c r="F38" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="58" t="s">
         <v>210</v>
       </c>
       <c r="B40" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="C40" t="s">
         <v>221</v>
       </c>
       <c r="D40" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="E40" t="s">
         <v>228</v>
@@ -3193,45 +3196,51 @@
       <c r="F40" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G40" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="58" t="s">
         <v>211</v>
       </c>
       <c r="B41" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C41" t="s">
         <v>227</v>
       </c>
       <c r="D41" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="E41" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F41" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+      <c r="G41" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="58" t="s">
         <v>212</v>
       </c>
       <c r="B42" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C42" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D42" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="E42" t="s">
+        <v>230</v>
+      </c>
+      <c r="F42" t="s">
         <v>231</v>
-      </c>
-      <c r="F42" t="s">
-        <v>232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Text formatting for dialogs (spaces and comas workarounds)
</commit_message>
<xml_diff>
--- a/Unstable/StarFighter/Documentation/Factions.xlsx
+++ b/Unstable/StarFighter/Documentation/Factions.xlsx
@@ -4,12 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Vanguard" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -1703,7 +1702,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V57"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="L24" sqref="L24:O38"/>
     </sheetView>
   </sheetViews>
@@ -2762,7 +2761,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
@@ -3247,16 +3246,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>